<commit_message>
Sd add new ms (#129)
* add MS manquants 3e1fec6cbbfd264868a0305e126b6218b14cb64b
</commit_message>
<xml_diff>
--- a/ig/main/StructureDefinition-eclaire-group.xlsx
+++ b/ig/main/StructureDefinition-eclaire-group.xlsx
@@ -9,6 +9,9 @@
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
     <sheet name="Elements" r:id="rId4" sheetId="2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="true">Elements!$A$1:$AL$34</definedName>
+  </definedNames>
 </workbook>
 </file>
 
@@ -54,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-02-16T15:42:28+00:00</t>
+    <t>2024-02-19T18:04:21+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1018,6 +1021,21 @@
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <bgColor indexed="22"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color indexed="22"/>
+        <i val="true"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -1356,7 +1374,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" hidden="true">
       <c r="A2" t="s" s="2">
         <v>29</v>
       </c>
@@ -1464,7 +1482,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" hidden="true">
       <c r="A3" t="s" s="2">
         <v>83</v>
       </c>
@@ -1572,7 +1590,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" hidden="true">
       <c r="A4" t="s" s="2">
         <v>91</v>
       </c>
@@ -1678,7 +1696,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" hidden="true">
       <c r="A5" t="s" s="2">
         <v>99</v>
       </c>
@@ -1786,7 +1804,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" hidden="true">
       <c r="A6" t="s" s="2">
         <v>106</v>
       </c>
@@ -1894,7 +1912,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" hidden="true">
       <c r="A7" t="s" s="2">
         <v>115</v>
       </c>
@@ -2002,7 +2020,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" hidden="true">
       <c r="A8" t="s" s="2">
         <v>123</v>
       </c>
@@ -2110,7 +2128,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" hidden="true">
       <c r="A9" t="s" s="2">
         <v>130</v>
       </c>
@@ -2218,7 +2236,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" hidden="true">
       <c r="A10" t="s" s="2">
         <v>141</v>
       </c>
@@ -2328,7 +2346,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" hidden="true">
       <c r="A11" t="s" s="2">
         <v>146</v>
       </c>
@@ -2436,7 +2454,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" hidden="true">
       <c r="A12" t="s" s="2">
         <v>153</v>
       </c>
@@ -2546,7 +2564,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
         <v>161</v>
       </c>
@@ -2656,7 +2674,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
         <v>171</v>
       </c>
@@ -2764,7 +2782,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
         <v>177</v>
       </c>
@@ -2872,7 +2890,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
         <v>186</v>
       </c>
@@ -2982,7 +3000,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
         <v>193</v>
       </c>
@@ -3092,7 +3110,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
         <v>200</v>
       </c>
@@ -3200,7 +3218,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
         <v>207</v>
       </c>
@@ -3310,7 +3328,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
         <v>214</v>
       </c>
@@ -3416,7 +3434,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
         <v>218</v>
       </c>
@@ -3524,7 +3542,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
         <v>221</v>
       </c>
@@ -3634,7 +3652,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
         <v>226</v>
       </c>
@@ -3653,7 +3671,7 @@
         <v>84</v>
       </c>
       <c r="H23" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I23" t="s" s="2">
         <v>74</v>
@@ -3742,7 +3760,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
         <v>233</v>
       </c>
@@ -3850,7 +3868,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
         <v>242</v>
       </c>
@@ -3871,7 +3889,7 @@
         <v>84</v>
       </c>
       <c r="H25" t="s" s="2">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="I25" t="s" s="2">
         <v>74</v>
@@ -3960,7 +3978,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
         <v>245</v>
       </c>
@@ -4070,7 +4088,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
         <v>251</v>
       </c>
@@ -4178,7 +4196,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
         <v>258</v>
       </c>
@@ -4286,7 +4304,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
         <v>263</v>
       </c>
@@ -4392,7 +4410,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
         <v>264</v>
       </c>
@@ -4500,7 +4518,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
         <v>265</v>
       </c>
@@ -4610,7 +4628,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
         <v>266</v>
       </c>
@@ -4718,7 +4736,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
         <v>271</v>
       </c>
@@ -4830,7 +4848,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
         <v>276</v>
       </c>
@@ -4941,6 +4959,24 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AL34">
+    <filterColumn colId="6">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <filterColumn colId="26">
+      <filters blank="true"/>
+    </filterColumn>
+  </autoFilter>
+  <conditionalFormatting sqref="A2:AI33">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$G2&lt;&gt;"Y"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$Q2&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>